<commit_message>
data analysis half of the data
</commit_message>
<xml_diff>
--- a/files/p03.xlsx
+++ b/files/p03.xlsx
@@ -431,7 +431,8 @@
       <sheetName val="participants"/>
       <sheetName val="inventory"/>
       <sheetName val="places"/>
-      <sheetName val="type"/>
+      <sheetName val="forms"/>
+      <sheetName val="activities"/>
       <sheetName val="all-items-raw"/>
       <sheetName val="places_copy"/>
       <sheetName val="participants_raw"/>
@@ -3837,6 +3838,7 @@
       <sheetData sheetId="26"/>
       <sheetData sheetId="27"/>
       <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -8367,8 +8369,8 @@
   <dimension ref="A1:AI200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C98" sqref="C98"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12755,15 +12757,15 @@
         <v>1.636574074074074E-2</v>
       </c>
       <c r="D97" s="5">
-        <v>1.6597222222222222E-2</v>
+        <v>1.6620370370370372E-2</v>
       </c>
       <c r="E97" s="5">
         <f t="shared" si="8"/>
-        <v>2.3148148148148182E-4</v>
+        <v>2.5462962962963243E-4</v>
       </c>
       <c r="F97" s="6">
         <f t="shared" si="9"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G97" s="6">
         <f t="shared" si="10"/>
@@ -12771,7 +12773,7 @@
       </c>
       <c r="H97" s="6">
         <f t="shared" si="11"/>
-        <v>1434</v>
+        <v>1436</v>
       </c>
       <c r="I97" s="1" t="str">
         <f>VLOOKUP(J97,'[1]all-items'!$A$2:$C$299,2,FALSE)</f>

</xml_diff>